<commit_message>
feat: Agregar selección de tipo de operación e ingreso en el formulario de DTEs
</commit_message>
<xml_diff>
--- a/public/reportes/formato_consumidor_final.xlsx
+++ b/public/reportes/formato_consumidor_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a967b2abe915b65f/Facturación Electrónica/Frontend/nuevo_dashboard/public/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{12C99E88-0B15-481E-8250-E261BFB4F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E847DB2B-A6C9-447A-8511-FC99ED969655}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{12C99E88-0B15-481E-8250-E261BFB4F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1ED15B9-0C24-4092-88E4-A19AF0374DEC}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B3A9F5CE-F22A-444E-AD6A-23DD2A0B849C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3A9F5CE-F22A-444E-AD6A-23DD2A0B849C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>FECHA</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Ventas Exentas:</t>
   </si>
   <si>
-    <t>Ventas Gravadas:</t>
-  </si>
-  <si>
     <t>Ventas Sin IVA:</t>
   </si>
   <si>
@@ -121,6 +118,15 @@
   </si>
   <si>
     <t>Ventas No Sujetas</t>
+  </si>
+  <si>
+    <t>Exportaciones 0%</t>
+  </si>
+  <si>
+    <t>Ventas Gravadas 13%:</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -264,12 +270,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,6 +282,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -598,168 +607,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED28B72A-4775-489F-A167-C6C95589A5F8}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.578125" customWidth="1"/>
-    <col min="8" max="8" width="19.41796875" customWidth="1"/>
-    <col min="9" max="9" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.26171875" customWidth="1"/>
-    <col min="11" max="11" width="16.41796875" customWidth="1"/>
-    <col min="12" max="12" width="23.83984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.68359375" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="10" t="s">
+      <c r="J9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="7" t="s">
+      <c r="L9" s="8"/>
+      <c r="M9" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -784,17 +793,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="5">
         <v>0</v>
       </c>
@@ -811,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L14" t="s">
         <v>21</v>
       </c>
@@ -820,58 +829,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="6">
         <f>I12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="6">
+        <f>K12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
         <v>22</v>
-      </c>
-      <c r="M16" s="6">
-        <f>SUM(K12:L12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="L17" t="s">
-        <v>23</v>
       </c>
       <c r="M17" s="6">
         <f>M16/1.13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" s="6">
         <f>M17*0.13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="8"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="12"/>
       <c r="L19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="13">
+        <f>L12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="15">
+        <f>M14+M15+M16-M19+M20</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A2:M2"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="J9:J10"/>
@@ -885,10 +916,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Actualizar formato de exportación de consumidores para incluir nuevos campos de control
</commit_message>
<xml_diff>
--- a/public/reportes/formato_consumidor_final.xlsx
+++ b/public/reportes/formato_consumidor_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a967b2abe915b65f/Facturación Electrónica/Frontend/nuevo_dashboard/public/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{12C99E88-0B15-481E-8250-E261BFB4F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1ED15B9-0C24-4092-88E4-A19AF0374DEC}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{12C99E88-0B15-481E-8250-E261BFB4F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58726C9F-5A69-4E44-8635-83C80D2A9304}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3A9F5CE-F22A-444E-AD6A-23DD2A0B849C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B3A9F5CE-F22A-444E-AD6A-23DD2A0B849C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>FECHA</t>
   </si>
@@ -66,9 +66,6 @@
     <t>TOTAL VENTAS</t>
   </si>
   <si>
-    <t>NUMERO DE DOCUMENTO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Del No. </t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>CÓDIGO DE GENERACIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NÚMERO DE CONTROL</t>
   </si>
 </sst>
 </file>
@@ -262,7 +265,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -270,6 +273,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,12 +297,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -607,168 +613,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED28B72A-4775-489F-A167-C6C95589A5F8}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.578125" customWidth="1"/>
+    <col min="8" max="10" width="19.41796875" customWidth="1"/>
+    <col min="11" max="11" width="19.26171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.26171875" customWidth="1"/>
+    <col min="13" max="13" width="16.41796875" customWidth="1"/>
+    <col min="14" max="14" width="23.83984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="13"/>
+      <c r="O9" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -777,12 +801,8 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="4">
         <v>0</v>
       </c>
@@ -792,130 +812,139 @@
       <c r="M11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N14" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
+      <c r="O14" s="6">
+        <f>L12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="6">
+        <f>K12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="6">
+        <f>M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N17" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="6">
-        <f>J12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L15" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="6">
-        <f>I12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="6">
-        <f>K12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="6">
-        <f>M16/1.13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="6">
+        <f>O16/1.13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="6">
+        <f>O17*0.13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="N19" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="6">
-        <f>M17*0.13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="13">
-        <f>L12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L21" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="15">
-        <f>M14+M15+M16-M19+M20</f>
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N20" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="8">
+        <f>N12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="N21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="10">
+        <f>O14+O15+O16-O19+O20</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:O1"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="L9:L10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>